<commit_message>
add data and code
add data and code for probit regression inflation rate
</commit_message>
<xml_diff>
--- a/inflation_data_18_23_new.xlsx
+++ b/inflation_data_18_23_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PENS\Semester 5\Ekonometrika\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1CFA27-D0A5-47B3-9EA0-2DFB912D39F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1920D448-F2B4-47A6-8D9D-7A092782C556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{34E9A701-9693-4063-94A4-3A23CCC20A36}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11280" xr2:uid="{34E9A701-9693-4063-94A4-3A23CCC20A36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t>m_to_m</t>
-  </si>
-  <si>
     <t>exchange_rate</t>
   </si>
   <si>
@@ -58,6 +55,9 @@
   </si>
   <si>
     <t>ihsg</t>
+  </si>
+  <si>
+    <t>month</t>
   </si>
 </sst>
 </file>
@@ -433,7 +433,7 @@
   <dimension ref="A1:G121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -450,25 +450,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>